<commit_message>
updated alex scheme and some gui refinements
</commit_message>
<xml_diff>
--- a/WatanyaPingTester/bin/Debug/data/alex_scheme.xlsx
+++ b/WatanyaPingTester/bin/Debug/data/alex_scheme.xlsx
@@ -250,9 +250,6 @@
     <t>169.254.1.51</t>
   </si>
   <si>
-    <t>169.254.1.53</t>
-  </si>
-  <si>
     <t>Al Alamin Gate</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>Mobinil Nubariya Rd Ant. 2</t>
   </si>
   <si>
-    <t>169.254.1.68</t>
-  </si>
-  <si>
     <t>169.254.1.70</t>
   </si>
   <si>
@@ -362,6 +356,12 @@
   </si>
   <si>
     <t>169.254.1.31</t>
+  </si>
+  <si>
+    <t>169.254.1.60</t>
+  </si>
+  <si>
+    <t>169.254.1.59</t>
   </si>
 </sst>
 </file>
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,71 +720,71 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" t="s">
-        <v>101</v>
-      </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1042,25 +1042,25 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s">
         <v>107</v>
       </c>
-      <c r="B15" t="s">
-        <v>109</v>
-      </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1180,25 +1180,25 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" t="s">
         <v>106</v>
       </c>
-      <c r="B21" t="s">
-        <v>108</v>
-      </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
         <v>54</v>
@@ -1468,10 +1468,10 @@
         <v>54</v>
       </c>
       <c r="E33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G33" t="s">
         <v>54</v>
@@ -1479,7 +1479,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
         <v>55</v>
@@ -1491,10 +1491,10 @@
         <v>55</v>
       </c>
       <c r="E34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G34" t="s">
         <v>55</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
         <v>56</v>
@@ -1514,10 +1514,10 @@
         <v>56</v>
       </c>
       <c r="E35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G35" t="s">
         <v>56</v>
@@ -1525,48 +1525,48 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1663,25 +1663,25 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1827,13 +1827,13 @@
         <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="D49" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="E49" t="s">
         <v>76</v>
@@ -1842,191 +1842,191 @@
         <v>76</v>
       </c>
       <c r="G49" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" t="s">
         <v>79</v>
       </c>
-      <c r="B50" t="s">
-        <v>80</v>
-      </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F50" t="s">
+        <v>78</v>
+      </c>
+      <c r="G50" t="s">
         <v>79</v>
-      </c>
-      <c r="F50" t="s">
-        <v>79</v>
-      </c>
-      <c r="G50" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="C51" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="E51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G51" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" t="s">
         <v>82</v>
       </c>
-      <c r="B52" t="s">
-        <v>84</v>
-      </c>
       <c r="C52" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D52" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E52" t="s">
+        <v>81</v>
+      </c>
+      <c r="F52" t="s">
+        <v>81</v>
+      </c>
+      <c r="G52" t="s">
         <v>82</v>
-      </c>
-      <c r="F52" t="s">
-        <v>82</v>
-      </c>
-      <c r="G52" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" t="s">
         <v>89</v>
       </c>
-      <c r="B55" t="s">
-        <v>91</v>
-      </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E55" t="s">
+        <v>87</v>
+      </c>
+      <c r="F55" t="s">
+        <v>87</v>
+      </c>
+      <c r="G55" t="s">
         <v>89</v>
-      </c>
-      <c r="F55" t="s">
-        <v>89</v>
-      </c>
-      <c r="G55" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" t="s">
         <v>90</v>
       </c>
-      <c r="B56" t="s">
-        <v>92</v>
-      </c>
       <c r="C56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E56" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" t="s">
+        <v>88</v>
+      </c>
+      <c r="G56" t="s">
         <v>90</v>
-      </c>
-      <c r="F56" t="s">
-        <v>90</v>
-      </c>
-      <c r="G56" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C57" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D57" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E57" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F57" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G57" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>